<commit_message>
US273410 Move common scmldap routines to be used with endevorrepldap to commonldap
</commit_message>
<xml_diff>
--- a/commonldap/SourceMinder_Product_Contacts.xlsx
+++ b/commonldap/SourceMinder_Product_Contacts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\scmldap\scmldap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\commonldap\commonldap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4048,8 +4048,8 @@
   <dimension ref="A1:J356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F214" sqref="F214"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E206" sqref="E206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,7 +4058,7 @@
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Fix handling of large DL memberships.
</commit_message>
<xml_diff>
--- a/commonldap/SourceMinder_Product_Contacts.xlsx
+++ b/commonldap/SourceMinder_Product_Contacts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="1150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="1151">
   <si>
     <t>PROD_NAME</t>
   </si>
@@ -3469,6 +3469,9 @@
   </si>
   <si>
     <t>macco01</t>
+  </si>
+  <si>
+    <t>PFRCH</t>
   </si>
 </sst>
 </file>
@@ -4321,8 +4324,8 @@
   <dimension ref="A1:J442"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="1" topLeftCell="A400" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E419" sqref="E419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16316,7 +16319,7 @@
         <v>12</v>
       </c>
       <c r="E419" t="s">
-        <v>1119</v>
+        <v>1150</v>
       </c>
       <c r="G419" t="s">
         <v>1148</v>

</xml_diff>

<commit_message>
Update processing for "inactive" and "retired" projects to be like "end of life"
</commit_message>
<xml_diff>
--- a/commonldap/SourceMinder_Product_Contacts.xlsx
+++ b/commonldap/SourceMinder_Product_Contacts.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4559" uniqueCount="1477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4559" uniqueCount="1478">
   <si>
     <t>Viewpoint CS</t>
   </si>
@@ -4458,6 +4458,9 @@
   </si>
   <si>
     <t>CSCR504/Chorus,Distributed Storage Chorus Role;CSCR702</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -4864,8 +4867,8 @@
   <dimension ref="A1:J575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A519" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F520" sqref="F520"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9854,7 +9857,7 @@
         <v>687</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>2</v>
+        <v>1477</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
US351873 Add github parsing for SourceMinder_Product_Contact
</commit_message>
<xml_diff>
--- a/commonldap/SourceMinder_Product_Contacts.xlsx
+++ b/commonldap/SourceMinder_Product_Contacts.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Product Contact Matrix" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Contact Matrix'!$A$1:$L$695</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Contact Matrix'!$A$1:$L$696</definedName>
   </definedNames>
   <calcPr calcId="171026"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5743" uniqueCount="1773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5750" uniqueCount="1778">
   <si>
     <t>PROD_NAME</t>
   </si>
@@ -5346,6 +5346,21 @@
   </si>
   <si>
     <t>CSCR809</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>bobsr01</t>
+  </si>
+  <si>
+    <t>github-isl-01.ca.com/WLA</t>
+  </si>
+  <si>
+    <t>Workload Automation</t>
+  </si>
+  <si>
+    <t>[{"PMFKEY":"bobsr01","TYPE":"Team","NAME":"Agents"},{"PMFKEY":"bobsr01","TYPE":"Repository","NAME":"ae"}]</t>
   </si>
 </sst>
 </file>
@@ -5383,7 +5398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5408,6 +5423,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5421,7 +5442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5461,6 +5482,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5776,11 +5800,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L695"/>
+  <dimension ref="A1:L696"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A678" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A679" sqref="A679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25593,34 +25617,34 @@
       </c>
     </row>
     <row r="679" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A679" s="5" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B679" s="5"/>
-      <c r="C679" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D679" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E679" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F679" s="5" t="s">
-        <v>1719</v>
-      </c>
-      <c r="G679" s="5" t="s">
-        <v>1720</v>
-      </c>
-      <c r="H679" s="5"/>
-      <c r="I679" s="5"/>
-      <c r="J679" s="5" t="s">
-        <v>1721</v>
+      <c r="A679" s="14" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B679" s="14"/>
+      <c r="C679" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D679" s="14" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E679" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F679" s="14" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G679" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="H679" s="14"/>
+      <c r="I679" s="14"/>
+      <c r="J679" s="14" t="s">
+        <v>1774</v>
       </c>
     </row>
     <row r="680" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A680" s="5" t="s">
-        <v>1722</v>
+        <v>1718</v>
       </c>
       <c r="B680" s="5"/>
       <c r="C680" s="5" t="s">
@@ -25633,143 +25657,138 @@
         <v>42</v>
       </c>
       <c r="F680" s="5" t="s">
-        <v>1723</v>
+        <v>1719</v>
       </c>
       <c r="G680" s="5" t="s">
-        <v>541</v>
+        <v>1720</v>
       </c>
       <c r="H680" s="5"/>
       <c r="I680" s="5"/>
       <c r="J680" s="5" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="681" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A681" s="5" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B681" s="5"/>
+      <c r="C681" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D681" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E681" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F681" s="5" t="s">
+        <v>1723</v>
+      </c>
+      <c r="G681" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="H681" s="5"/>
+      <c r="I681" s="5"/>
+      <c r="J681" s="5" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="681" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A681" s="3" t="s">
+    <row r="682" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A682" s="3" t="s">
         <v>1724</v>
       </c>
-      <c r="B681" s="3" t="s">
+      <c r="B682" s="3" t="s">
         <v>1725</v>
       </c>
-      <c r="C681" s="3" t="s">
+      <c r="C682" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D681" s="3" t="s">
+      <c r="D682" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E681" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F681" s="3" t="s">
+      <c r="E682" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F682" s="3" t="s">
         <v>1726</v>
       </c>
-      <c r="G681" s="3" t="s">
+      <c r="G682" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H681" s="3"/>
-      <c r="I681" s="3"/>
-      <c r="J681" s="3" t="s">
+      <c r="H682" s="3"/>
+      <c r="I682" s="3"/>
+      <c r="J682" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="K681" s="3" t="s">
+      <c r="K682" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="682" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A682" s="5" t="s">
+    <row r="683" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A683" s="5" t="s">
         <v>1727</v>
       </c>
-      <c r="B682" s="5" t="s">
+      <c r="B683" s="5" t="s">
         <v>1728</v>
       </c>
-      <c r="C682" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D682" s="5" t="s">
+      <c r="C683" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D683" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E682" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F682" s="5" t="s">
+      <c r="E683" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F683" s="5" t="s">
         <v>1729</v>
       </c>
-      <c r="G682" s="5" t="s">
+      <c r="G683" s="5" t="s">
         <v>1730</v>
       </c>
-      <c r="H682" s="5"/>
-      <c r="I682" s="5" t="s">
+      <c r="H683" s="5"/>
+      <c r="I683" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J682" s="5" t="s">
+      <c r="J683" s="5" t="s">
         <v>1731</v>
       </c>
     </row>
-    <row r="683" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A683" s="2" t="s">
+    <row r="684" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A684" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="B683" s="2" t="s">
+      <c r="B684" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C683" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D683" s="2" t="s">
+      <c r="C684" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D684" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E683" s="2" t="s">
+      <c r="E684" s="2" t="s">
         <v>1734</v>
       </c>
-      <c r="F683" s="2" t="s">
+      <c r="F684" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G683" s="2" t="s">
+      <c r="G684" s="2" t="s">
         <v>1735</v>
       </c>
-      <c r="H683" s="2"/>
-      <c r="I683" s="2"/>
-      <c r="J683" s="2" t="s">
+      <c r="H684" s="2"/>
+      <c r="I684" s="2"/>
+      <c r="J684" s="2" t="s">
         <v>1736</v>
       </c>
     </row>
-    <row r="684" spans="1:12" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A684" s="3" t="s">
+    <row r="685" spans="1:12" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A685" s="3" t="s">
         <v>1732</v>
       </c>
-      <c r="B684" s="3" t="s">
+      <c r="B685" s="3" t="s">
         <v>1733</v>
-      </c>
-      <c r="C684" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D684" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E684" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F684" s="3" t="s">
-        <v>1737</v>
-      </c>
-      <c r="G684" s="3" t="s">
-        <v>1735</v>
-      </c>
-      <c r="H684" s="3"/>
-      <c r="I684" s="3"/>
-      <c r="J684" s="3" t="s">
-        <v>1736</v>
-      </c>
-      <c r="K684" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="685" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A685" s="3" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B685" s="3">
-        <v>2.4</v>
       </c>
       <c r="C685" s="3" t="s">
         <v>13</v>
@@ -25781,7 +25800,7 @@
         <v>42</v>
       </c>
       <c r="F685" s="3" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="G685" s="3" t="s">
         <v>1735</v>
@@ -25796,188 +25815,195 @@
       </c>
     </row>
     <row r="686" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A686" s="2" t="s">
+      <c r="A686" s="3" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B686" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="C686" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D686" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E686" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F686" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="G686" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="H686" s="3"/>
+      <c r="I686" s="3"/>
+      <c r="J686" s="3" t="s">
+        <v>1736</v>
+      </c>
+      <c r="K686" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="687" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A687" s="2" t="s">
         <v>1740</v>
       </c>
-      <c r="B686" s="2">
+      <c r="B687" s="2">
         <v>3.1</v>
       </c>
-      <c r="C686" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D686" s="2" t="s">
+      <c r="C687" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D687" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E686" s="2" t="s">
+      <c r="E687" s="2" t="s">
         <v>1734</v>
       </c>
-      <c r="F686" s="2" t="s">
+      <c r="F687" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G686" s="2" t="s">
+      <c r="G687" s="2" t="s">
         <v>1741</v>
       </c>
-      <c r="H686" s="2"/>
-      <c r="I686" s="2" t="s">
+      <c r="H687" s="2"/>
+      <c r="I687" s="2" t="s">
         <v>1224</v>
       </c>
-      <c r="J686" s="2" t="s">
+      <c r="J687" s="2" t="s">
         <v>1742</v>
       </c>
     </row>
-    <row r="687" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A687" s="3" t="s">
+    <row r="688" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A688" s="3" t="s">
         <v>1743</v>
       </c>
-      <c r="B687" s="3" t="s">
+      <c r="B688" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="C687" s="3" t="s">
+      <c r="C688" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D687" s="3" t="s">
+      <c r="D688" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E687" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F687" s="3" t="s">
+      <c r="E688" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F688" s="3" t="s">
         <v>1744</v>
       </c>
-      <c r="G687" s="3" t="s">
+      <c r="G688" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H687" s="3"/>
-      <c r="I687" s="3"/>
-      <c r="J687" s="3" t="s">
+      <c r="H688" s="3"/>
+      <c r="I688" s="3"/>
+      <c r="J688" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="K687" s="3" t="s">
+      <c r="K688" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="688" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A688" s="2" t="s">
+    <row r="689" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A689" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="B688" s="2" t="s">
+      <c r="B689" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C688" s="2" t="s">
+      <c r="C689" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D688" s="2" t="s">
+      <c r="D689" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E688" s="2" t="s">
+      <c r="E689" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F688" s="2" t="s">
+      <c r="F689" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G688" s="2" t="s">
+      <c r="G689" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H688" s="2"/>
-      <c r="I688" s="2"/>
-      <c r="J688" s="2" t="s">
+      <c r="H689" s="2"/>
+      <c r="I689" s="2"/>
+      <c r="J689" s="2" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="689" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A689" s="3" t="s">
-        <v>1745</v>
-      </c>
-      <c r="B689" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C689" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D689" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E689" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F689" s="3" t="s">
-        <v>1746</v>
-      </c>
-      <c r="G689" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H689" s="3"/>
-      <c r="I689" s="3"/>
-      <c r="J689" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K689" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="690" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A690" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B690" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C690" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D690" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E690" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F690" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="G690" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H690" s="3"/>
+      <c r="I690" s="3"/>
+      <c r="J690" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K690" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="691" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A691" s="3" t="s">
         <v>1747</v>
       </c>
-      <c r="B690" s="3" t="s">
+      <c r="B691" s="3" t="s">
         <v>1317</v>
       </c>
-      <c r="C690" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D690" s="3" t="s">
+      <c r="C691" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D691" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="E690" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F690" s="3" t="s">
+      <c r="E691" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F691" s="3" t="s">
         <v>1748</v>
       </c>
-      <c r="G690" s="3" t="s">
+      <c r="G691" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H690" s="3"/>
-      <c r="I690" s="3" t="s">
+      <c r="H691" s="3"/>
+      <c r="I691" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="J690" s="3" t="s">
+      <c r="J691" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K690" s="3" t="s">
+      <c r="K691" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="L690" s="3" t="s">
+      <c r="L691" s="3" t="s">
         <v>1749</v>
-      </c>
-    </row>
-    <row r="691" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A691" s="2" t="s">
-        <v>1750</v>
-      </c>
-      <c r="B691" s="2"/>
-      <c r="C691" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D691" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E691" s="2" t="s">
-        <v>1750</v>
-      </c>
-      <c r="F691" s="2"/>
-      <c r="G691" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H691" s="2"/>
-      <c r="I691" s="2"/>
-      <c r="J691" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="692" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A692" s="2" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B692" s="2"/>
       <c r="C692" s="2" t="s">
@@ -25987,86 +26013,82 @@
         <v>14</v>
       </c>
       <c r="E692" s="2" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="F692" s="2"/>
       <c r="G692" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H692" s="2"/>
       <c r="I692" s="2"/>
       <c r="J692" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="693" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A693" s="2" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B693" s="2"/>
+      <c r="C693" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D693" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E693" s="2" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F693" s="2"/>
+      <c r="G693" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H693" s="2"/>
+      <c r="I693" s="2"/>
+      <c r="J693" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="693" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A693" s="3" t="s">
+    <row r="694" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A694" s="3" t="s">
         <v>1752</v>
       </c>
-      <c r="B693" s="3" t="s">
+      <c r="B694" s="3" t="s">
         <v>1753</v>
       </c>
-      <c r="C693" s="3" t="s">
+      <c r="C694" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D693" s="3" t="s">
+      <c r="D694" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E693" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F693" s="3" t="s">
+      <c r="E694" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F694" s="3" t="s">
         <v>1754</v>
       </c>
-      <c r="G693" s="3" t="s">
+      <c r="G694" s="3" t="s">
         <v>1473</v>
       </c>
-      <c r="H693" s="3" t="s">
+      <c r="H694" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="I693" s="3"/>
-      <c r="J693" s="3" t="s">
+      <c r="I694" s="3"/>
+      <c r="J694" s="3" t="s">
         <v>1474</v>
       </c>
-      <c r="K693" s="3" t="s">
+      <c r="K694" s="3" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="694" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A694" s="5" t="s">
-        <v>1771</v>
-      </c>
-      <c r="B694" s="5"/>
-      <c r="C694" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D694" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E694" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F694" s="5" t="s">
-        <v>1772</v>
-      </c>
-      <c r="G694" s="5" t="s">
-        <v>1758</v>
-      </c>
-      <c r="H694" s="5"/>
-      <c r="I694" s="5" t="s">
-        <v>1224</v>
-      </c>
-      <c r="J694" s="5" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="695" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A695" s="5" t="s">
-        <v>1755</v>
+        <v>1771</v>
       </c>
       <c r="B695" s="5"/>
       <c r="C695" s="5" t="s">
-        <v>205</v>
+        <v>13</v>
       </c>
       <c r="D695" s="5" t="s">
         <v>47</v>
@@ -26075,14 +26097,42 @@
         <v>42</v>
       </c>
       <c r="F695" s="5" t="s">
+        <v>1772</v>
+      </c>
+      <c r="G695" s="5" t="s">
+        <v>1758</v>
+      </c>
+      <c r="H695" s="5"/>
+      <c r="I695" s="5" t="s">
+        <v>1224</v>
+      </c>
+      <c r="J695" s="5" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="696" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A696" s="5" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B696" s="5"/>
+      <c r="C696" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D696" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E696" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F696" s="5" t="s">
         <v>1770</v>
       </c>
-      <c r="G695" s="5" t="s">
+      <c r="G696" s="5" t="s">
         <v>1756</v>
       </c>
-      <c r="H695" s="5"/>
-      <c r="I695" s="5"/>
-      <c r="J695" s="5" t="s">
+      <c r="H696" s="5"/>
+      <c r="I696" s="5"/>
+      <c r="J696" s="5" t="s">
         <v>1757</v>
       </c>
     </row>
@@ -26093,6 +26143,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -26142,46 +26201,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Order0 xmlns="afd34d76-bd0a-4401-a24d-7f289c41d043">1</Order0>
-    <SharedWithUsers xmlns="caa4e187-f897-484e-8238-9cf00fcb7318">
-      <UserInfo>
-        <DisplayName>Costello, Debra L</DisplayName>
-        <AccountId>8430</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Bigornia Jr, Agustin</DisplayName>
-        <AccountId>11541</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Armstrong, Francis J</DisplayName>
-        <AccountId>9317</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Morales, John</DisplayName>
-        <AccountId>316</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0E9129E47F7CB438C96AC380E87590A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e88feaa25e6ad09e6ba324897e71446">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="caa4e187-f897-484e-8238-9cf00fcb7318" xmlns:ns3="afd34d76-bd0a-4401-a24d-7f289c41d043" xmlns:ns4="a875d3b0-e276-4560-a424-4019c376e5e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f03fa3b171511b141aa43c09ca253c1" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="caa4e187-f897-484e-8238-9cf00fcb7318"/>
@@ -26359,7 +26379,45 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Order0 xmlns="afd34d76-bd0a-4401-a24d-7f289c41d043">1</Order0>
+    <SharedWithUsers xmlns="caa4e187-f897-484e-8238-9cf00fcb7318">
+      <UserInfo>
+        <DisplayName>Costello, Debra L</DisplayName>
+        <AccountId>8430</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Bigornia Jr, Agustin</DisplayName>
+        <AccountId>11541</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Armstrong, Francis J</DisplayName>
+        <AccountId>9317</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Morales, John</DisplayName>
+        <AccountId>316</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F157CC7-0BC4-4431-8527-4D48F8B34954}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8654B897-6565-4D9A-AEDC-2108E98326EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -26367,33 +26425,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F157CC7-0BC4-4431-8527-4D48F8B34954}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B6277B-C863-49C0-93F5-52BF35BF4D15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="caa4e187-f897-484e-8238-9cf00fcb7318"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a875d3b0-e276-4560-a424-4019c376e5e2"/>
-    <ds:schemaRef ds:uri="afd34d76-bd0a-4401-a24d-7f289c41d043"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668497AE-C76A-4CE9-8BAA-F6F3316D1975}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26411,4 +26443,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B6277B-C863-49C0-93F5-52BF35BF4D15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="caa4e187-f897-484e-8238-9cf00fcb7318"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a875d3b0-e276-4560-a424-4019c376e5e2"/>
+    <ds:schemaRef ds:uri="afd34d76-bd0a-4401-a24d-7f289c41d043"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Master.  Commit changes to Product Contacts
</commit_message>
<xml_diff>
--- a/commonldap/SourceMinder_Product_Contacts.xlsx
+++ b/commonldap/SourceMinder_Product_Contacts.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5801" uniqueCount="1794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5798" uniqueCount="1794">
   <si>
     <t>PROD_NAME</t>
   </si>
@@ -5496,7 +5496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5555,6 +5555,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18033,12 +18036,10 @@
         <v>13</v>
       </c>
       <c r="D422" s="15"/>
-      <c r="E422" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F422" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="E422" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F422" s="15"/>
       <c r="G422" s="15" t="s">
         <v>1783</v>
       </c>
@@ -19218,9 +19219,7 @@
       <c r="E463" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F463" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="F463" s="15"/>
       <c r="G463" s="15" t="s">
         <v>1783</v>
       </c>
@@ -24163,9 +24162,7 @@
       <c r="E631" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F631" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="F631" s="15"/>
       <c r="G631" s="15" t="s">
         <v>1783</v>
       </c>
@@ -26396,15 +26393,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Order0 xmlns="afd34d76-bd0a-4401-a24d-7f289c41d043">1</Order0>
@@ -26434,7 +26422,66 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0E9129E47F7CB438C96AC380E87590A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e88feaa25e6ad09e6ba324897e71446">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="caa4e187-f897-484e-8238-9cf00fcb7318" xmlns:ns3="afd34d76-bd0a-4401-a24d-7f289c41d043" xmlns:ns4="a875d3b0-e276-4560-a424-4019c376e5e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f03fa3b171511b141aa43c09ca253c1" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="caa4e187-f897-484e-8238-9cf00fcb7318"/>
@@ -26612,65 +26659,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F157CC7-0BC4-4431-8527-4D48F8B34954}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B6277B-C863-49C0-93F5-52BF35BF4D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -26688,7 +26677,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F157CC7-0BC4-4431-8527-4D48F8B34954}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8654B897-6565-4D9A-AEDC-2108E98326EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668497AE-C76A-4CE9-8BAA-F6F3316D1975}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26706,12 +26711,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8654B897-6565-4D9A-AEDC-2108E98326EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add production credentials to ticketing process
</commit_message>
<xml_diff>
--- a/commonldap/SourceMinder_Product_Contacts.xlsx
+++ b/commonldap/SourceMinder_Product_Contacts.xlsx
@@ -27001,7 +27001,101 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0E9129E47F7CB438C96AC380E87590A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39995d888827efcf204ab0c3dc3774cb">
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Order0 xmlns="afd34d76-bd0a-4401-a24d-7f289c41d043">1</Order0>
+    <SharedWithUsers xmlns="caa4e187-f897-484e-8238-9cf00fcb7318">
+      <UserInfo>
+        <DisplayName>Costello, Debra L</DisplayName>
+        <AccountId>8430</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Bigornia Jr, Agustin</DisplayName>
+        <AccountId>11541</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Armstrong, Francis J</DisplayName>
+        <AccountId>9317</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Morales, John</DisplayName>
+        <AccountId>316</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Beriau, Bernie R</DisplayName>
+        <AccountId>4457</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0E9129E47F7CB438C96AC380E87590A" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="62825a3371e69d163f9638d6c6be3376">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="caa4e187-f897-484e-8238-9cf00fcb7318" xmlns:ns3="afd34d76-bd0a-4401-a24d-7f289c41d043" xmlns:ns4="a875d3b0-e276-4560-a424-4019c376e5e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89b1f1d2fccfd2d7e23e03ab43ea116e" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="caa4e187-f897-484e-8238-9cf00fcb7318"/>
     <xsd:import namespace="afd34d76-bd0a-4401-a24d-7f289c41d043"/>
@@ -27190,102 +27284,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8654B897-6565-4D9A-AEDC-2108E98326EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F157CC7-0BC4-4431-8527-4D48F8B34954}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Order0 xmlns="afd34d76-bd0a-4401-a24d-7f289c41d043">1</Order0>
-    <SharedWithUsers xmlns="caa4e187-f897-484e-8238-9cf00fcb7318">
-      <UserInfo>
-        <DisplayName>Costello, Debra L</DisplayName>
-        <AccountId>8430</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Bigornia Jr, Agustin</DisplayName>
-        <AccountId>11541</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Armstrong, Francis J</DisplayName>
-        <AccountId>9317</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Morales, John</DisplayName>
-        <AccountId>316</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Beriau, Bernie R</DisplayName>
-        <AccountId>4457</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B6277B-C863-49C0-93F5-52BF35BF4D15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a875d3b0-e276-4560-a424-4019c376e5e2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="afd34d76-bd0a-4401-a24d-7f289c41d043"/>
+    <ds:schemaRef ds:uri="caa4e187-f897-484e-8238-9cf00fcb7318"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7400E32-D5BC-41E6-B73C-359CF80FD9CF}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35308FA4-18F5-43BE-B53B-FB5410CCBC34}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -27302,38 +27336,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8654B897-6565-4D9A-AEDC-2108E98326EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F157CC7-0BC4-4431-8527-4D48F8B34954}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B6277B-C863-49C0-93F5-52BF35BF4D15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="caa4e187-f897-484e-8238-9cf00fcb7318"/>
-    <ds:schemaRef ds:uri="a875d3b0-e276-4560-a424-4019c376e5e2"/>
-    <ds:schemaRef ds:uri="afd34d76-bd0a-4401-a24d-7f289c41d043"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>